<commit_message>
Add the first of multiple citation functions.
</commit_message>
<xml_diff>
--- a/inst/extdata/docs/notes.xlsx
+++ b/inst/extdata/docs/notes.xlsx
@@ -108,43 +108,43 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,23 +450,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27" style="10" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -475,16 +475,16 @@
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the latex cite functions
</commit_message>
<xml_diff>
--- a/inst/extdata/docs/notes.xlsx
+++ b/inst/extdata/docs/notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Gist/Quote</t>
   </si>
@@ -31,6 +31,21 @@
   </si>
   <si>
     <t>Document (bib key)</t>
+  </si>
+  <si>
+    <t>rinker2013</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>An **EXAMPLE**; feel "free" to *delete* it ***soon**</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>EXAMPLE (DELETE ME)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +465,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,11 +495,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed a bug that occurs from reading in quotes with `gdata:::read.xlsx`
</commit_message>
<xml_diff>
--- a/inst/extdata/docs/notes.xlsx
+++ b/inst/extdata/docs/notes.xlsx
@@ -39,13 +39,13 @@
     <t>12</t>
   </si>
   <si>
-    <t>An **EXAMPLE**; feel "free" to *delete* it ***soon**</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
     <t>EXAMPLE (DELETE ME)</t>
+  </si>
+  <si>
+    <t>An **EXAMPLE**; feel "free" to *delete* it ***soon***</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,13 +502,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fix to read.notes compliments of mathematical.coffee:
http://stackoverflow.com/a/15939139/1000343

close #20
</commit_message>
<xml_diff>
--- a/inst/extdata/docs/notes.xlsx
+++ b/inst/extdata/docs/notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Gist/Quote</t>
   </si>
@@ -46,13 +46,79 @@
   </si>
   <si>
     <t>An **EXAMPLE**; feel "free" to *delete* it ***soon***</t>
+  </si>
+  <si>
+    <t>en dash</t>
+  </si>
+  <si>
+    <t>em dash</t>
+  </si>
+  <si>
+    <t>&amp;agrave;</t>
+  </si>
+  <si>
+    <t>à</t>
+  </si>
+  <si>
+    <t>&amp;aacute;</t>
+  </si>
+  <si>
+    <t>&amp;egrave;</t>
+  </si>
+  <si>
+    <t>&amp;eacute;</t>
+  </si>
+  <si>
+    <t>common markup symbols</t>
+  </si>
+  <si>
+    <t>equiv</t>
+  </si>
+  <si>
+    <t>á</t>
+  </si>
+  <si>
+    <t>é</t>
+  </si>
+  <si>
+    <t>è</t>
+  </si>
+  <si>
+    <t>&amp;ndash;</t>
+  </si>
+  <si>
+    <t>&amp;mdash;</t>
+  </si>
+  <si>
+    <t>&amp;ouml;</t>
+  </si>
+  <si>
+    <t>ö</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>italics</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>curly quotes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,8 +126,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +149,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -121,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -160,6 +238,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,11 +549,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,9 +563,11 @@
     <col min="3" max="3" width="51.5703125" style="12" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" style="12" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -493,8 +583,14 @@
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -509,6 +605,84 @@
       </c>
       <c r="E2" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates notes to show -- and ---
</commit_message>
<xml_diff>
--- a/inst/extdata/docs/notes.xlsx
+++ b/inst/extdata/docs/notes.xlsx
@@ -84,12 +84,6 @@
     <t>è</t>
   </si>
   <si>
-    <t>&amp;ndash;</t>
-  </si>
-  <si>
-    <t>&amp;mdash;</t>
-  </si>
-  <si>
     <t>&amp;ouml;</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>curly quotes</t>
+  </si>
+  <si>
+    <t>&amp;ndash;    or     --</t>
+  </si>
+  <si>
+    <t>&amp;mdash;    or    ---</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>10</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G3" s="16" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>11</v>
@@ -655,34 +655,34 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G9" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G10" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G11" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced gdata as the xlsx importer with package xlsx.  Also notes has been renamed to notes_reportnam.csv/xls
close #21
close #22
</commit_message>
<xml_diff>
--- a/inst/extdata/docs/notes.xlsx
+++ b/inst/extdata/docs/notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Gist/Quote</t>
   </si>
@@ -112,13 +112,63 @@
   </si>
   <si>
     <t>&amp;mdash;    or    ---</t>
+  </si>
+  <si>
+    <t>Q column stands for quote</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mark with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">y </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(yes)-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(no)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +178,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,12 +208,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -158,8 +218,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F05A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -195,29 +261,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -229,7 +296,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -242,18 +309,35 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF8F05A"/>
+      <color rgb="FFFFFF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -549,140 +633,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G3"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27" style="6" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="12" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>